<commit_message>
working on player bio walkon music player
</commit_message>
<xml_diff>
--- a/bio/player_bio.xlsx
+++ b/bio/player_bio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matevass/Documents/Programming/R/darts-statistics/bio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C8B909-8D8F-2648-A3DC-CDCE74946406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72ACF82-59EA-6949-A4DF-0D2E3B1AC298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -100,55 +100,55 @@
     <t>Szvetaki</t>
   </si>
   <si>
+    <t>19g Harrows Voodoo</t>
+  </si>
+  <si>
+    <t>Tomi Csánk</t>
+  </si>
+  <si>
+    <t>Fubu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bee Gees - Stayin' Alive </t>
+  </si>
+  <si>
+    <t>22g Harrows Blaze</t>
+  </si>
+  <si>
+    <t>Dani Pusztai</t>
+  </si>
+  <si>
+    <t>The President</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bellini - Samba de Janeiro </t>
+  </si>
+  <si>
+    <t>Ármin Szücs</t>
+  </si>
+  <si>
+    <t>The Jag</t>
+  </si>
+  <si>
+    <t>Kenny Loggins - Danger Zone</t>
+  </si>
+  <si>
+    <t>Zsombor Gulácsi</t>
+  </si>
+  <si>
+    <t>Márk Sipos</t>
+  </si>
+  <si>
+    <t>Darts Used</t>
+  </si>
+  <si>
+    <t>Date of Birth</t>
+  </si>
+  <si>
+    <t>Career 180s</t>
+  </si>
+  <si>
     <t>The Killers - Mr. Brightside</t>
-  </si>
-  <si>
-    <t>19g Harrows Voodoo</t>
-  </si>
-  <si>
-    <t>Tomi Csánk</t>
-  </si>
-  <si>
-    <t>Fubu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bee Gees - Stayin' Alive </t>
-  </si>
-  <si>
-    <t>22g Harrows Blaze</t>
-  </si>
-  <si>
-    <t>Dani Pusztai</t>
-  </si>
-  <si>
-    <t>The President</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bellini - Samba de Janeiro </t>
-  </si>
-  <si>
-    <t>Ármin Szücs</t>
-  </si>
-  <si>
-    <t>The Jag</t>
-  </si>
-  <si>
-    <t>Kenny Loggins - Danger Zone</t>
-  </si>
-  <si>
-    <t>Zsombor Gulácsi</t>
-  </si>
-  <si>
-    <t>Márk Sipos</t>
-  </si>
-  <si>
-    <t>Darts Used</t>
-  </si>
-  <si>
-    <t>Date of Birth</t>
-  </si>
-  <si>
-    <t>Career 180s</t>
   </si>
 </sst>
 </file>
@@ -518,7 +518,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -544,7 +544,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
@@ -553,10 +553,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -689,7 +689,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="D7" s="6">
         <v>36533</v>
@@ -701,7 +701,7 @@
         <v>9</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H7" s="7">
         <v>0</v>
@@ -709,13 +709,13 @@
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="D8" s="6">
         <v>36485</v>
@@ -727,7 +727,7 @@
         <v>9</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H8" s="7">
         <v>0</v>
@@ -735,13 +735,13 @@
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="C9" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>34</v>
       </c>
       <c r="D9" s="6">
         <v>38962</v>
@@ -758,13 +758,13 @@
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="C10" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>37</v>
       </c>
       <c r="D10" s="6">
         <v>35864</v>
@@ -781,7 +781,7 @@
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="6">
@@ -799,7 +799,7 @@
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>

</xml_diff>

<commit_message>
added walk-on music for everybody
</commit_message>
<xml_diff>
--- a/bio/player_bio.xlsx
+++ b/bio/player_bio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matevass/Documents/Programming/R/darts-statistics/bio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72ACF82-59EA-6949-A4DF-0D2E3B1AC298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C4C5CF-73BC-AC4A-A268-5A593736B195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="49">
   <si>
     <t>Player</t>
   </si>
@@ -85,9 +85,6 @@
     <t>Vaya Con Dios - Nah Neh Nah</t>
   </si>
   <si>
-    <t>20g (idk)</t>
-  </si>
-  <si>
     <t>Bálint Bakos</t>
   </si>
   <si>
@@ -109,9 +106,6 @@
     <t>Fubu</t>
   </si>
   <si>
-    <t xml:space="preserve">Bee Gees - Stayin' Alive </t>
-  </si>
-  <si>
     <t>22g Harrows Blaze</t>
   </si>
   <si>
@@ -149,6 +143,30 @@
   </si>
   <si>
     <t>The Killers - Mr. Brightside</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bee Gees - Stayin Alive </t>
+  </si>
+  <si>
+    <t>20g</t>
+  </si>
+  <si>
+    <t>Guli</t>
+  </si>
+  <si>
+    <t>Sipi</t>
+  </si>
+  <si>
+    <t>Ivan &amp; The Parazol - Take My Hand</t>
+  </si>
+  <si>
+    <t>Bëlga - Rendőrmunka</t>
+  </si>
+  <si>
+    <t>Groovehouse - Vándor</t>
+  </si>
+  <si>
+    <t>No information available</t>
   </si>
 </sst>
 </file>
@@ -518,14 +536,14 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
@@ -544,7 +562,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
@@ -553,10 +571,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -604,6 +622,9 @@
       <c r="F3" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="G3" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="H3" s="7">
         <v>1</v>
       </c>
@@ -654,7 +675,7 @@
         <v>9</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="H5" s="7">
         <v>0</v>
@@ -662,12 +683,14 @@
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="5"/>
+      <c r="C6" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="D6" s="6">
         <v>36337</v>
       </c>
@@ -677,19 +700,22 @@
       <c r="F6" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="G6" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="H6" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="C7" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D7" s="6">
         <v>36533</v>
@@ -701,7 +727,7 @@
         <v>9</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H7" s="7">
         <v>0</v>
@@ -709,13 +735,13 @@
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>28</v>
-      </c>
       <c r="C8" s="5" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="D8" s="6">
         <v>36485</v>
@@ -727,7 +753,7 @@
         <v>9</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H8" s="7">
         <v>0</v>
@@ -735,13 +761,13 @@
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>33</v>
       </c>
       <c r="D9" s="6">
         <v>38962</v>
@@ -752,19 +778,22 @@
       <c r="F9" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="G9" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="H9" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="D10" s="6">
         <v>35864</v>
@@ -775,15 +804,23 @@
       <c r="F10" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="G10" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="H10" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="5"/>
+        <v>35</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="D11" s="6">
         <v>36439</v>
       </c>
@@ -793,16 +830,23 @@
       <c r="F11" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="G11" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="H11" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
+        <v>36</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>47</v>
+      </c>
       <c r="D12" s="10">
         <v>36230</v>
       </c>
@@ -812,7 +856,9 @@
       <c r="F12" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="9"/>
+      <c r="G12" s="9" t="s">
+        <v>48</v>
+      </c>
       <c r="H12" s="11">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
added 2025 round 1 results
</commit_message>
<xml_diff>
--- a/bio/player_bio.xlsx
+++ b/bio/player_bio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matevass/Documents/Programming/R/darts-statistics/bio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE195AA-129B-5C49-99D3-9399B5F360FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7034110-54AA-2643-B9AF-6823268C5A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
   <si>
     <t>Player</t>
   </si>
@@ -136,9 +136,6 @@
     <t xml:space="preserve">Bee Gees - Stayin Alive </t>
   </si>
   <si>
-    <t>20g</t>
-  </si>
-  <si>
     <t>Guli</t>
   </si>
   <si>
@@ -151,9 +148,6 @@
     <t>Groovehouse - Vándor</t>
   </si>
   <si>
-    <t>No information available</t>
-  </si>
-  <si>
     <t>Pitbull</t>
   </si>
   <si>
@@ -176,6 +170,21 @@
   </si>
   <si>
     <t>23g Red Dragon Fury 2</t>
+  </si>
+  <si>
+    <t>21g Bulls</t>
+  </si>
+  <si>
+    <t>20g Decathlon</t>
+  </si>
+  <si>
+    <t>Geri Vass</t>
+  </si>
+  <si>
+    <t>Balázs Pápai</t>
+  </si>
+  <si>
+    <t>Baja</t>
   </si>
 </sst>
 </file>
@@ -207,27 +216,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -242,9 +236,11 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
@@ -259,7 +255,7 @@
         <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom/>
@@ -268,22 +264,33 @@
     <border>
       <left/>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color rgb="FF000000"/>
-      </left>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -292,18 +299,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -311,19 +307,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,10 +540,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -561,314 +559,348 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="11" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="3">
         <v>36217</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="3">
         <v>36337</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="3">
+        <v>36298</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H3" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="6">
-        <v>36298</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="3">
+        <v>36371</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="3">
+        <v>37068</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="3">
+        <v>36533</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="3">
+        <v>36485</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="3">
+        <v>38962</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="3">
+        <v>35864</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H4" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="6">
-        <v>36371</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="5" t="s">
+      <c r="H10" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="H5" s="7">
+      <c r="C11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="3">
+        <v>36439</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="6">
-        <v>37068</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="H6" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="6">
-        <v>36533</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="H7" s="7">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="5">
+        <v>36230</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="6">
-        <v>36485</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="H8" s="7">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="5">
+        <v>37437</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="6"/>
+      <c r="H13" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="6">
-        <v>38962</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="H9" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="6">
-        <v>35864</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H10" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="6">
-        <v>36439</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H11" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="10">
-        <v>36230</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="H12" s="11">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="13"/>
+      <c r="H14" s="12">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated new player bios
</commit_message>
<xml_diff>
--- a/bio/player_bio.xlsx
+++ b/bio/player_bio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matevass/Documents/Programming/R/darts-statistics/bio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7034110-54AA-2643-B9AF-6823268C5A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804258E1-548C-6045-9D54-408DDFCEB2A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="54">
   <si>
     <t>Player</t>
   </si>
@@ -182,9 +182,6 @@
   </si>
   <si>
     <t>Balázs Pápai</t>
-  </si>
-  <si>
-    <t>Baja</t>
   </si>
 </sst>
 </file>
@@ -307,21 +304,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,7 +537,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -559,7 +553,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -580,12 +574,12 @@
       <c r="G1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="7" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -606,12 +600,12 @@
       <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="9">
+      <c r="H2" s="6">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -632,12 +626,12 @@
       <c r="G3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -658,12 +652,12 @@
       <c r="G4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -684,12 +678,12 @@
       <c r="G5" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -710,12 +704,12 @@
       <c r="G6" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="6">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -736,12 +730,12 @@
       <c r="G7" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -762,12 +756,12 @@
       <c r="G8" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -788,12 +782,12 @@
       <c r="G9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -814,12 +808,12 @@
       <c r="G10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -838,69 +832,69 @@
         <v>9</v>
       </c>
       <c r="G11" s="2"/>
-      <c r="H11" s="9">
+      <c r="H11" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="3">
         <v>36230</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="9">
+      <c r="E12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="3">
         <v>37437</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="10">
+      <c r="E13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" s="13"/>
-      <c r="H14" s="12">
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="10">
+        <v>36552</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="9"/>
+      <c r="H14" s="8">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added 2025 round 2 results
</commit_message>
<xml_diff>
--- a/bio/player_bio.xlsx
+++ b/bio/player_bio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matevass/Documents/Programming/R/darts-statistics/bio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804258E1-548C-6045-9D54-408DDFCEB2A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C4F239-DFED-D740-871A-B1CBC9045A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -537,7 +537,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -705,7 +705,7 @@
         <v>45</v>
       </c>
       <c r="H6" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
added new walkon song
</commit_message>
<xml_diff>
--- a/bio/player_bio.xlsx
+++ b/bio/player_bio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matevass/Documents/Programming/R/darts-statistics/bio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C4F239-DFED-D740-871A-B1CBC9045A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47697DAC-5F1C-014F-8E3B-6785E9A23379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
   <si>
     <t>Player</t>
   </si>
@@ -182,6 +182,9 @@
   </si>
   <si>
     <t>Balázs Pápai</t>
+  </si>
+  <si>
+    <t>Johannes Brahms - Hungarian Dance No. 5 in G Minor</t>
   </si>
 </sst>
 </file>
@@ -537,14 +540,14 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
@@ -883,7 +886,9 @@
         <v>53</v>
       </c>
       <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
+      <c r="C14" s="9" t="s">
+        <v>54</v>
+      </c>
       <c r="D14" s="10">
         <v>36552</v>
       </c>

</xml_diff>

<commit_message>
added new walk-on song
</commit_message>
<xml_diff>
--- a/bio/player_bio.xlsx
+++ b/bio/player_bio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matevass/Documents/Programming/R/darts-statistics/bio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47697DAC-5F1C-014F-8E3B-6785E9A23379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2C4BAA-31BF-A640-A79E-C9D79679AFE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="58">
   <si>
     <t>Player</t>
   </si>
@@ -185,6 +185,15 @@
   </si>
   <si>
     <t>Johannes Brahms - Hungarian Dance No. 5 in G Minor</t>
+  </si>
+  <si>
+    <t>Jayron, GEWOONRAVES - Knock Knock</t>
+  </si>
+  <si>
+    <t>Baja</t>
+  </si>
+  <si>
+    <t>Papito</t>
   </si>
 </sst>
 </file>
@@ -540,7 +549,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -867,6 +876,12 @@
       <c r="A13" s="6" t="s">
         <v>52</v>
       </c>
+      <c r="B13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" t="s">
+        <v>55</v>
+      </c>
       <c r="D13" s="3">
         <v>37437</v>
       </c>
@@ -885,7 +900,9 @@
       <c r="A14" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="9"/>
+      <c r="B14" s="9" t="s">
+        <v>56</v>
+      </c>
       <c r="C14" s="9" t="s">
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
changed a walk-on song
</commit_message>
<xml_diff>
--- a/bio/player_bio.xlsx
+++ b/bio/player_bio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matevass/Documents/Programming/R/darts-statistics/bio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2C4BAA-31BF-A640-A79E-C9D79679AFE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6CE3DD5-CA44-D746-9F70-991D9B597092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -187,13 +187,13 @@
     <t>Johannes Brahms - Hungarian Dance No. 5 in G Minor</t>
   </si>
   <si>
-    <t>Jayron, GEWOONRAVES - Knock Knock</t>
-  </si>
-  <si>
     <t>Baja</t>
   </si>
   <si>
     <t>Papito</t>
+  </si>
+  <si>
+    <t>Orishas - A Lo Cubano</t>
   </si>
 </sst>
 </file>
@@ -549,7 +549,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -877,10 +877,10 @@
         <v>52</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" t="s">
         <v>57</v>
-      </c>
-      <c r="C13" t="s">
-        <v>55</v>
       </c>
       <c r="D13" s="3">
         <v>37437</v>
@@ -901,7 +901,7 @@
         <v>53</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
fixed player not participated in this season error
</commit_message>
<xml_diff>
--- a/bio/player_bio.xlsx
+++ b/bio/player_bio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matevass/Documents/Programming/R/darts-statistics/bio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6CE3DD5-CA44-D746-9F70-991D9B597092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB2B2C3-7F46-D04A-B79F-D87CC32D8AE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="59">
   <si>
     <t>Player</t>
   </si>
@@ -194,6 +194,9 @@
   </si>
   <si>
     <t>Orishas - A Lo Cubano</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -549,7 +552,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -843,7 +846,9 @@
       <c r="F11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="H11" s="6">
         <v>0</v>
       </c>
@@ -867,7 +872,9 @@
       <c r="F12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="H12" s="6">
         <v>0</v>
       </c>
@@ -891,7 +898,9 @@
       <c r="F13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="2"/>
+      <c r="G13" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="H13" s="6">
         <v>0</v>
       </c>
@@ -915,7 +924,9 @@
       <c r="F14" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="9"/>
+      <c r="G14" s="9" t="s">
+        <v>58</v>
+      </c>
       <c r="H14" s="8">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
added 2025 round 5 results and fixed bugs
</commit_message>
<xml_diff>
--- a/bio/player_bio.xlsx
+++ b/bio/player_bio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matevass/Documents/Programming/R/darts-statistics/bio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778158F1-60D6-8E48-9C36-0900BBE14FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE42E0D-F2CA-C246-A252-850724BB5B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="62">
   <si>
     <t>Player</t>
   </si>
@@ -76,9 +76,6 @@
     <t>Laci Ferenczi</t>
   </si>
   <si>
-    <t>Darcbalynok</t>
-  </si>
-  <si>
     <t>Vaya Con Dios - Nah Neh Nah</t>
   </si>
   <si>
@@ -197,6 +194,18 @@
   </si>
   <si>
     <t>Papacito</t>
+  </si>
+  <si>
+    <t>Parittyás</t>
+  </si>
+  <si>
+    <t>Feri Gyulai-Nagy</t>
+  </si>
+  <si>
+    <t>Feri</t>
+  </si>
+  <si>
+    <t>Gwen Stefani, Akon - The Sweet Escape</t>
   </si>
 </sst>
 </file>
@@ -229,7 +238,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -316,11 +325,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -329,8 +347,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -550,10 +570,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -579,7 +599,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -588,10 +608,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -640,7 +660,7 @@
         <v>9</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H3" s="6">
         <v>1</v>
@@ -666,7 +686,7 @@
         <v>9</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H4" s="6">
         <v>5</v>
@@ -677,10 +697,10 @@
         <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="D5" s="3">
         <v>36371</v>
@@ -692,21 +712,21 @@
         <v>9</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H5" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="D6" s="3">
         <v>37068</v>
@@ -718,7 +738,7 @@
         <v>9</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H6" s="6">
         <v>4</v>
@@ -726,13 +746,13 @@
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" s="3">
         <v>36533</v>
@@ -744,7 +764,7 @@
         <v>9</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H7" s="6">
         <v>0</v>
@@ -752,13 +772,13 @@
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="C8" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="3">
         <v>36485</v>
@@ -770,7 +790,7 @@
         <v>9</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H8" s="6">
         <v>0</v>
@@ -778,13 +798,13 @@
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="D9" s="3">
         <v>38962</v>
@@ -796,7 +816,7 @@
         <v>9</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H9" s="6">
         <v>0</v>
@@ -804,13 +824,13 @@
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="D10" s="3">
         <v>35864</v>
@@ -822,7 +842,7 @@
         <v>9</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H10" s="6">
         <v>0</v>
@@ -830,13 +850,13 @@
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11" s="3">
         <v>36439</v>
@@ -848,7 +868,7 @@
         <v>9</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H11" s="6">
         <v>0</v>
@@ -856,13 +876,13 @@
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D12" s="3">
         <v>36230</v>
@@ -874,7 +894,7 @@
         <v>9</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H12" s="6">
         <v>0</v>
@@ -882,13 +902,13 @@
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" s="3">
         <v>37437</v>
@@ -900,35 +920,61 @@
         <v>9</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H13" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" s="10">
+      <c r="D14" s="3">
         <v>36552</v>
       </c>
-      <c r="E14" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="H14" s="8">
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="12">
+        <v>39597</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="H15" s="9">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added 2025 round 8 results
</commit_message>
<xml_diff>
--- a/bio/player_bio.xlsx
+++ b/bio/player_bio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matevass/Documents/Programming/R/darts-statistics/bio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E345B255-6A7E-784E-AE89-6D08A0F5B662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0491889D-BB30-7648-97B4-48577762627A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="620" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -183,9 +183,6 @@
     <t>21g Bulls</t>
   </si>
   <si>
-    <t>20g Decathlon</t>
-  </si>
-  <si>
     <t>Geri Vass</t>
   </si>
   <si>
@@ -232,6 +229,9 @@
   </si>
   <si>
     <t>Dani Boldizsár</t>
+  </si>
+  <si>
+    <t>20g One80 Dragon</t>
   </si>
 </sst>
 </file>
@@ -600,7 +600,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -690,7 +690,7 @@
         <v>45</v>
       </c>
       <c r="H3" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -724,7 +724,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>18</v>
@@ -739,10 +739,10 @@
         <v>9</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="H5" s="6">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -872,7 +872,7 @@
         <v>49</v>
       </c>
       <c r="H10" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -895,7 +895,7 @@
         <v>9</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H11" s="6">
         <v>0</v>
@@ -921,7 +921,7 @@
         <v>9</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H12" s="6">
         <v>0</v>
@@ -929,13 +929,13 @@
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D13" s="3">
         <v>37437</v>
@@ -947,7 +947,7 @@
         <v>9</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H13" s="6">
         <v>0</v>
@@ -955,13 +955,13 @@
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" t="s">
         <v>52</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" t="s">
-        <v>53</v>
       </c>
       <c r="D14" s="3">
         <v>36552</v>
@@ -973,7 +973,7 @@
         <v>9</v>
       </c>
       <c r="G14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H14" s="6">
         <v>0</v>
@@ -981,13 +981,13 @@
     </row>
     <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="C15" t="s">
         <v>60</v>
-      </c>
-      <c r="C15" t="s">
-        <v>61</v>
       </c>
       <c r="D15" s="3">
         <v>39597</v>
@@ -999,7 +999,7 @@
         <v>9</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H15" s="6">
         <v>1</v>
@@ -1007,13 +1007,13 @@
     </row>
     <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B16" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>63</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>64</v>
       </c>
       <c r="D16" s="13">
         <v>36412</v>
@@ -1025,10 +1025,10 @@
         <v>9</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H16" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added 2025 round 10 results
</commit_message>
<xml_diff>
--- a/bio/player_bio.xlsx
+++ b/bio/player_bio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matevass/Documents/Programming/R/darts-statistics/bio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9A4692-91B9-B243-BC68-0EDD7BBB6173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3706CF77-5307-4D41-8897-029806605368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="620" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -600,7 +600,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -742,7 +742,7 @@
         <v>66</v>
       </c>
       <c r="H5" s="6">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>